<commit_message>
Export to excel function completed.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\cstsang\workspace\rosterWeb_react_node\server\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cstsang\workspace\roster_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B2E6B1-02FE-4792-9A85-B6C88D9466FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EABA1E-51EF-4625-819C-522E8EADA415}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2070" yWindow="4200" windowWidth="23250" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -440,7 +440,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -555,6 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -936,7 +937,7 @@
   <dimension ref="A1:AQ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1286,6 +1287,11 @@
       <c r="Z8" s="31"/>
       <c r="AA8" s="31"/>
       <c r="AB8" s="31"/>
+      <c r="AC8" s="42"/>
+      <c r="AD8" s="42"/>
+      <c r="AE8" s="42"/>
+      <c r="AF8" s="42"/>
+      <c r="AG8" s="42"/>
     </row>
     <row r="9" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -1320,6 +1326,10 @@
       <c r="Z9" s="31"/>
       <c r="AA9" s="31"/>
       <c r="AB9" s="31"/>
+      <c r="AC9" s="42"/>
+      <c r="AD9" s="42"/>
+      <c r="AE9" s="42"/>
+      <c r="AF9" s="42"/>
     </row>
     <row r="10" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
@@ -1629,14 +1639,14 @@
   <mergeCells count="10">
     <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S8:AB8"/>
-    <mergeCell ref="S9:AB9"/>
     <mergeCell ref="B1:AF1"/>
     <mergeCell ref="AG4:AK4"/>
     <mergeCell ref="AG5:AG6"/>
     <mergeCell ref="AH5:AH6"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="B2:AF2"/>
+    <mergeCell ref="S8:AG8"/>
+    <mergeCell ref="S9:AF9"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>